<commit_message>
sustitucion region code por nombre de provincias
</commit_message>
<xml_diff>
--- a/Recursos/cod_provincias.xlsx
+++ b/Recursos/cod_provincias.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlando/Documents/GitHub/TFM-EasyMoney/Recursos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{498F20D4-7BEA-9641-A882-D234F420CC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED8936C-58DA-C042-979D-8F44E5212E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2620" windowWidth="27640" windowHeight="16940" xr2:uid="{EE15D4F5-9A5B-B249-B5C1-E985049B238A}"/>
+    <workbookView xWindow="60" yWindow="2880" windowWidth="27640" windowHeight="16940" xr2:uid="{EE15D4F5-9A5B-B249-B5C1-E985049B238A}"/>
   </bookViews>
   <sheets>
     <sheet name="COD PROVINCIAS" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'COD PROVINCIAS'!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,15 +62,9 @@
     <t>04</t>
   </si>
   <si>
-    <t>Almería</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
-    <t>Álava</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>05</t>
   </si>
   <si>
-    <t>Ávila</t>
-  </si>
-  <si>
     <t>06</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>07</t>
   </si>
   <si>
-    <t>Baleares</t>
-  </si>
-  <si>
     <t>08</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>48</t>
   </si>
   <si>
-    <t>Bizkaia</t>
-  </si>
-  <si>
     <t>09</t>
   </si>
   <si>
@@ -113,15 +101,9 @@
     <t>10</t>
   </si>
   <si>
-    <t>Cáceres</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
-    <t>Cádiz</t>
-  </si>
-  <si>
     <t>39</t>
   </si>
   <si>
@@ -131,9 +113,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>Castellón</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
@@ -143,15 +122,9 @@
     <t>14</t>
   </si>
   <si>
-    <t>Córdoba</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
-    <t>Coruña</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -161,15 +134,9 @@
     <t>20</t>
   </si>
   <si>
-    <t>Gipuzkoa</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
-    <t>Girona</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -197,21 +164,12 @@
     <t>23</t>
   </si>
   <si>
-    <t>Jaén</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
-    <t>León</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
-    <t>Lleida</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -227,9 +185,6 @@
     <t>29</t>
   </si>
   <si>
-    <t>Málaga</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
@@ -245,9 +200,6 @@
     <t>32</t>
   </si>
   <si>
-    <t>Ourense</t>
-  </si>
-  <si>
     <t>34</t>
   </si>
   <si>
@@ -257,9 +209,6 @@
     <t>35</t>
   </si>
   <si>
-    <t>Palmas</t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
@@ -269,9 +218,6 @@
     <t>26</t>
   </si>
   <si>
-    <t>Rioja</t>
-  </si>
-  <si>
     <t>37</t>
   </si>
   <si>
@@ -281,9 +227,6 @@
     <t>38</t>
   </si>
   <si>
-    <t>Tenerife</t>
-  </si>
-  <si>
     <t>40</t>
   </si>
   <si>
@@ -354,13 +297,73 @@
   </si>
   <si>
     <t>Melilla</t>
+  </si>
+  <si>
+    <t>Alava</t>
+  </si>
+  <si>
+    <t>Almeria</t>
+  </si>
+  <si>
+    <t>Avila</t>
+  </si>
+  <si>
+    <t>Islas Baleares</t>
+  </si>
+  <si>
+    <t>Caceres</t>
+  </si>
+  <si>
+    <t>Cadiz</t>
+  </si>
+  <si>
+    <t>Castellon</t>
+  </si>
+  <si>
+    <t>Cordoba</t>
+  </si>
+  <si>
+    <t>La Coruña</t>
+  </si>
+  <si>
+    <t>Gerona</t>
+  </si>
+  <si>
+    <t>Guipuzcoa</t>
+  </si>
+  <si>
+    <t>Jaen</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>Lerida</t>
+  </si>
+  <si>
+    <t>La Rioja</t>
+  </si>
+  <si>
+    <t>Malaga</t>
+  </si>
+  <si>
+    <t>Orense</t>
+  </si>
+  <si>
+    <t>Las Palmas</t>
+  </si>
+  <si>
+    <t>Santa Cruz de Tenerife</t>
+  </si>
+  <si>
+    <t>Vizcaya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -376,10 +379,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -402,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -410,9 +425,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,439 +764,499 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28654819-24FE-2E4F-9A3E-44DF8599A2E9}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="B2" sqref="B2:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="B49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="D53" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{28654819-24FE-2E4F-9A3E-44DF8599A2E9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
+      <sortCondition ref="A1:A53"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>